<commit_message>
Reorganised excel data files and reduced the number of states and actions included within these files
</commit_message>
<xml_diff>
--- a/PredatorRewards.xlsx
+++ b/PredatorRewards.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD732D-FA12-4FD6-9BED-1D13664DDB9E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B4A988-FDB9-4596-80EF-37FAAA1DE3B0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>NO_PRED</t>
   </si>
   <si>
-    <t>NO_PREDIDLE</t>
-  </si>
-  <si>
     <t>NO_PREDRAND</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>NO_PREDFLEE</t>
   </si>
   <si>
-    <t>NEAR_PREDIDLE</t>
-  </si>
-  <si>
     <t>NEAR_PREDRAND</t>
   </si>
   <si>
@@ -53,9 +47,6 @@
   </si>
   <si>
     <t>NEAR_PREDFLEE</t>
-  </si>
-  <si>
-    <t>BEING_EATENIDLE</t>
   </si>
   <si>
     <t>BEING_EATENRAND</t>
@@ -391,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,10 +401,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -463,10 +454,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.99</v>
+        <v>-0.99</v>
       </c>
       <c r="C5">
-        <v>-0.5</v>
+        <v>-0.99</v>
       </c>
       <c r="D5">
         <v>-0.99</v>
@@ -477,10 +468,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.99</v>
+        <v>0.99</v>
       </c>
       <c r="C6">
-        <v>-0.99</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>-0.99</v>
@@ -519,10 +510,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.99</v>
+        <v>0.5</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
         <v>-0.99</v>
@@ -536,7 +527,7 @@
         <v>0.99</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D10">
         <v>-0.99</v>
@@ -547,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.99</v>
       </c>
       <c r="C11">
         <v>0.5</v>
@@ -578,51 +569,9 @@
         <v>0.99</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0.99</v>
       </c>
       <c r="D13">
-        <v>-0.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.99</v>
-      </c>
-      <c r="C14">
-        <v>0.5</v>
-      </c>
-      <c r="D14">
-        <v>-0.99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.99</v>
-      </c>
-      <c r="C15">
-        <v>0.5</v>
-      </c>
-      <c r="D15">
-        <v>-0.99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0.99</v>
-      </c>
-      <c r="C16">
-        <v>0.99</v>
-      </c>
-      <c r="D16">
         <v>-0.99</v>
       </c>
     </row>

</xml_diff>